<commit_message>
add id blog post
</commit_message>
<xml_diff>
--- a/public/blog/data_mgmt_resources/resources.xlsx
+++ b/public/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325B5A93-56D2-4AE1-BEDE-BD77EEDAA87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA5936A-4C2A-430A-B3AD-59BF830C1C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="110">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -341,9 +341,6 @@
     <t xml:space="preserve">&lt;a href="https://forrt.org/glossary/open-science/"&gt;FORRT Glossary&lt;/a&gt;; &lt;a href="https://open-science-training-handbook.gitbook.io/book/glossary"&gt;Open Science Training Handbook Glossary&lt;/a&gt;; &lt;a href="https://dataflowtoolkit.dk/process.php?otypeid=120"&gt;Data Flow Toolkit Processes&lt;/a&gt;; &lt;a href="https://irb.ucsf.edu/definitions"&gt;UCSF HRPP Definitions&lt;/a&gt;; &lt;a href="https://data.research.cornell.edu/content/glossary"&gt;Cornell University Glossary of data management terms&lt;/a&gt;; </t>
   </si>
   <si>
-    <t>J-Pal</t>
-  </si>
-  <si>
     <t>&lt;a href="https://www.povertyactionlab.org/resource/data-cleaning-and-management"&gt;Data cleaning and management&lt;/a&gt;</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
     <t>Borghi, J., Abrams, S., Lowenberg, D., Simms, S. &amp; Chodacki, J.</t>
   </si>
   <si>
-    <t>&lt;a href="https://doi.org/10.3897/rio.4.e26439"&gt;Promoting Open Science Through Research Data Management&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Johns Hopkins Institute for Clinical and Translational Research (ICTR)</t>
   </si>
   <si>
@@ -366,6 +360,18 @@
   </si>
   <si>
     <t>&lt;a href="https://www.povertyactionlab.org/resource/introduction-randomized-evaluations"&gt;Research Resources&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Dupriez, O., Sanchez Castro, M. &amp;  Revision, M.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://guide-for-data-archivists.readthedocs.io/en/latest/introduction.html"&gt;Guide for Data Archivists&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://doi.org/10.3897/rio.4.e26439"&gt;Support Your Data: A Research Data Management Guide for Researchers&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>J-Pal*</t>
   </si>
 </sst>
 </file>
@@ -722,13 +728,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -736,7 +742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -744,7 +750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -752,7 +758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -760,15 +766,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -776,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -784,15 +790,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -800,7 +806,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -832,13 +838,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.453125" customWidth="1"/>
-    <col min="2" max="2" width="64.81640625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -846,7 +852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -854,7 +860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -862,7 +868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -870,7 +876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -878,7 +884,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -886,7 +892,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -894,7 +900,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -902,7 +908,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -937,13 +943,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="33.54296875" customWidth="1"/>
-    <col min="3" max="3" width="170.7265625" customWidth="1"/>
+    <col min="1" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="170.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -954,7 +960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -965,7 +971,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -976,7 +982,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -987,18 +993,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>2018</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1020,7 +1026,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1053,7 +1059,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1104,13 +1110,13 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1160,13 +1166,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1190,7 +1196,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1237,13 +1243,13 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1267,7 +1273,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -1275,7 +1281,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1283,15 +1289,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1326,19 +1332,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1354,7 +1360,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1370,7 +1376,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1378,96 +1384,105 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
       <c r="B9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
         <v>99</v>
       </c>
-      <c r="B10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
       <c r="B12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>78</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>82</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
-    <sortCondition ref="A2:A14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
+    <sortCondition ref="A2:A15"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
-    <hyperlink ref="B9" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{BF5DB17B-A2E9-4364-9EA8-EAFDC95D0D19}"/>
+    <hyperlink ref="B9" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
+    <hyperlink ref="B10" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{BF5DB17B-A2E9-4364-9EA8-EAFDC95D0D19}"/>
     <hyperlink ref="B5" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B7E8A39-208D-4BAB-BD0E-C476EEF71874}"/>
     <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{17FB9F7C-2EEB-420C-AD50-8F5369FBC4E8}"/>
     <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8736C4FB-ED40-4AAA-A513-1B3997C412A1}"/>
-    <hyperlink ref="B11" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
-    <hyperlink ref="B7" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
+    <hyperlink ref="B12" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
     <hyperlink ref="B3" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{6400C49C-6A30-43A4-8FD2-3A23E629EA75}"/>
-    <hyperlink ref="B13" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{7497676C-A29B-4896-B50B-F18E6702CD8C}"/>
-    <hyperlink ref="B14" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{58B0795A-28FC-46B1-AAC3-E406B300BDA2}"/>
-    <hyperlink ref="B6" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
-    <hyperlink ref="B12" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
-    <hyperlink ref="B10" r:id="rId13" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
+    <hyperlink ref="B14" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{7497676C-A29B-4896-B50B-F18E6702CD8C}"/>
+    <hyperlink ref="B15" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{58B0795A-28FC-46B1-AAC3-E406B300BDA2}"/>
+    <hyperlink ref="B7" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
+    <hyperlink ref="B11" r:id="rId13" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
+    <hyperlink ref="B6" r:id="rId14" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove r for rest
</commit_message>
<xml_diff>
--- a/public/blog/data_mgmt_resources/resources.xlsx
+++ b/public/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA5936A-4C2A-430A-B3AD-59BF830C1C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C68F9C0-42CF-43FE-931B-90B33CCAB152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="checklists" sheetId="5" r:id="rId5"/>
     <sheet name="other_resources" sheetId="6" r:id="rId6"/>
     <sheet name="data_cleaning" sheetId="7" r:id="rId7"/>
+    <sheet name="equity" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -332,9 +333,6 @@
     <t>&lt;a href="https://trace.tennessee.edu/cgi/viewcontent.cgi?article=1023&amp;context=utk_libpub"&gt;What Could Possibly Go Wrong? The Impact of Poor Data Management&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href="https://cghlewis.github.io/mpsi-data-training/training_6.html#Checklists"&gt;Checklists&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Glossaries</t>
   </si>
   <si>
@@ -372,6 +370,51 @@
   </si>
   <si>
     <t>J-Pal*</t>
+  </si>
+  <si>
+    <t>Urban Institute</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.urban.org/research/publication/do-no-harm-guide-applying-equity-awareness-data-privacy-methods"&gt;Do No Harm Guide: Applying Equity Awareness In Data Privacy Methods &lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Mathematica</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.mathematica.org/features/tips-for-conducting-equitable-and-culturally-responsive-evaluation"&gt;Tips for conducting equitable and culturally responsive evaluation&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.urban.org/sites/default/files/publication/102346/principles-for-advancing-equitable-data-practice_0.pdf"&gt;Principles for advancing equitable data practice&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Chicago Beyond</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://chicagobeyond.org/wp-content/uploads/2019/05/ChicagoBeyond_2019Guidebook.pdf"&gt;Why am I always being researched?&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Poverty Action Lab</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.povertyactionlab.org/resource/ethical-conduct-randomized-evaluations"&gt;Ethical conduct of randomized evaluations&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Lewis, C.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://cghlewis.com/talk/sssp_ecf/"&gt;10 Common Data Management Mistakes&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://cghlewis.com/talk/uhcl/"&gt;Data Management Workflows for Education Research Studies&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal Lewis </t>
+  </si>
+  <si>
+    <t>&lt;a href="https://cghlewis.com/blog/data_clean_01/"&gt;Data Cleaning for Data Sharing&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://drive.google.com/drive/folders/1lRKEx_uMhbzcLeVZZBPX6_amde5uYuvf"&gt;Checklists&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -729,12 +772,12 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -742,7 +785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -750,7 +793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -758,7 +801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -766,15 +809,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -782,7 +825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -790,15 +833,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
         <v>102</v>
       </c>
-      <c r="B8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -806,7 +849,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -838,13 +881,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
+    <col min="1" max="1" width="57.453125" customWidth="1"/>
+    <col min="2" max="2" width="64.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -852,7 +895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -860,7 +903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -868,7 +911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -876,7 +919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -884,7 +927,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -892,7 +935,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -900,7 +943,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -908,7 +951,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -943,13 +986,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="170.7109375" customWidth="1"/>
+    <col min="1" max="2" width="33.54296875" customWidth="1"/>
+    <col min="3" max="3" width="170.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -960,7 +1003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -971,7 +1014,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -982,7 +1025,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -993,18 +1036,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5">
         <v>2018</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1058,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1026,7 +1069,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1037,7 +1080,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1048,7 +1091,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1059,7 +1102,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1070,7 +1113,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1104,19 +1147,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E314F75B-5804-4835-9447-15ECE75CB0EC}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1124,35 +1167,53 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{F9369E95-DB00-415B-9C4E-26398D2D43ED}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{DB660BFF-32D8-4552-ADE1-A22912433FF8}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{57D36F4D-5ECB-424B-8CAE-D6BD44420EF1}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{DB660BFF-32D8-4552-ADE1-A22912433FF8}"/>
+    <hyperlink ref="B6" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{57D36F4D-5ECB-424B-8CAE-D6BD44420EF1}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{F9369E95-DB00-415B-9C4E-26398D2D43ED}"/>
+    <hyperlink ref="B3" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{31BEDC47-DAD5-48A5-9285-FE7C7BAF828A}"/>
+    <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{F2BB4DDC-F382-4471-AE08-8FFB6600BC49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1162,17 +1223,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF00AE3-BFD4-438F-8990-251D0720E643}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1180,15 +1241,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1196,7 +1257,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1204,7 +1265,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1212,7 +1273,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1243,13 +1304,13 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1257,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1265,7 +1326,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1273,15 +1334,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
         <v>97</v>
       </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1289,15 +1350,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1305,7 +1366,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1332,19 +1393,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1352,7 +1413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1360,7 +1421,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1368,7 +1429,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1376,7 +1437,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1384,105 +1445,191 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
         <v>106</v>
       </c>
-      <c r="B6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>88</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>63</v>
       </c>
       <c r="B10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>71</v>
       </c>
       <c r="B13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>78</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>82</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
-    <sortCondition ref="A2:A15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
-    <hyperlink ref="B10" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{BF5DB17B-A2E9-4364-9EA8-EAFDC95D0D19}"/>
+    <hyperlink ref="B10" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
+    <hyperlink ref="B11" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{BF5DB17B-A2E9-4364-9EA8-EAFDC95D0D19}"/>
     <hyperlink ref="B5" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B7E8A39-208D-4BAB-BD0E-C476EEF71874}"/>
     <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{17FB9F7C-2EEB-420C-AD50-8F5369FBC4E8}"/>
     <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8736C4FB-ED40-4AAA-A513-1B3997C412A1}"/>
-    <hyperlink ref="B12" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
+    <hyperlink ref="B13" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
     <hyperlink ref="B3" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{6400C49C-6A30-43A4-8FD2-3A23E629EA75}"/>
-    <hyperlink ref="B14" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{7497676C-A29B-4896-B50B-F18E6702CD8C}"/>
-    <hyperlink ref="B15" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{58B0795A-28FC-46B1-AAC3-E406B300BDA2}"/>
-    <hyperlink ref="B7" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
-    <hyperlink ref="B11" r:id="rId13" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
-    <hyperlink ref="B6" r:id="rId14" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
+    <hyperlink ref="B15" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{7497676C-A29B-4896-B50B-F18E6702CD8C}"/>
+    <hyperlink ref="B16" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{58B0795A-28FC-46B1-AAC3-E406B300BDA2}"/>
+    <hyperlink ref="B8" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
+    <hyperlink ref="B12" r:id="rId13" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
+    <hyperlink ref="B7" r:id="rId14" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
+    <hyperlink ref="B6" r:id="rId15" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537A38A0-57C3-4EAB-A64C-3AABAA2535FC}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.81640625" customWidth="1"/>
+    <col min="2" max="2" width="42.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B6">
+    <sortCondition ref="A2:A6"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{786A9D6B-B356-4524-94ED-5B4EC166CB79}"/>
+    <hyperlink ref="B6" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{D37DB090-50D1-4805-BC58-DDE1ECA07F90}"/>
+    <hyperlink ref="B3" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{96C0C26D-F87A-4D9B-A72D-7660D30A7053}"/>
+    <hyperlink ref="B2" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{D7C3013B-9776-48DC-A52E-0E1D14308CFB}"/>
+    <hyperlink ref="B4" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{E014BFA3-3EDC-4F5B-9A11-FDECDAE0284E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new blog post
</commit_message>
<xml_diff>
--- a/public/blog/data_mgmt_resources/resources.xlsx
+++ b/public/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C68F9C0-42CF-43FE-931B-90B33CCAB152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5943AD0-C51D-4071-BC05-143EE1AE805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="136">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Institute of Education Sciences</t>
   </si>
   <si>
-    <t>Crystal Lewis</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -64,18 +61,12 @@
     <t>&lt;a href="https://rdmkit.elixir-europe.org/"&gt;Research Data Management Kit&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href="https://the-turing-way.netlify.app/welcome"&gt;Guide&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href="https://ies.ed.gov/ncee/pubs/2022004/pdf/2022004.pdf"&gt;Sharing Study Data: A Guide for Education Researchers&lt;/a&gt;</t>
   </si>
   <si>
     <t>&lt;a href="https://www.icpsr.umich.edu/files/deposit/dataprep.pdf"&gt;Guide to Social Science Data Preparation and Archiving&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href="https://cghlewis.github.io/mpsi-data-training/index.html"&gt;Data Management in Large-Scale Education Research&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -181,9 +172,6 @@
     <t>&lt;a href="https://figshare.com/articles/presentation/Data_Sharing_and_Data_Shared/15040740"&gt;Data Sharing and Data Shared&lt;/a&gt;</t>
   </si>
   <si>
-    <t>All slides available from Kristin Briney</t>
-  </si>
-  <si>
     <t>&lt;a href="https://www.slideshare.net/kbriney?utm_campaign=profiletracking&amp;utm_medium=sssite&amp;utm_source=ssslideview"&gt;Kristin Briney Slide Share&lt;/a&gt;</t>
   </si>
   <si>
@@ -205,9 +193,6 @@
     <t>&lt;a href="https://datamanagement.hms.harvard.edu/about/what-research-data-management/biomedical-data-lifecycle"&gt;Research Data Management Checklist&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Kristin Briney</t>
-  </si>
-  <si>
     <t>&lt;a href="https://figshare.com/articles/poster/Data_Management_Plan_Checklist/1130852"&gt;Data Management Plan Checklist&lt;/a&gt;</t>
   </si>
   <si>
@@ -241,9 +226,6 @@
     <t>&lt;a href="https://povertyaction.github.io/guides/cleaning/readme/"&gt;Cleaning Guide&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href="https://cghlewis.github.io/mpsi-data-training/training_4.html"&gt;Data Cleaning Plan&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Broman, K. &amp; Woo, K.</t>
   </si>
   <si>
@@ -254,9 +236,6 @@
   </si>
   <si>
     <t>&lt;a href="https://www.acaps.org/sites/acaps/files/resources/files/acaps_technical_brief_data_cleaning_april_2016_0.pdf"&gt;Data Cleaning&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Karl Broman</t>
   </si>
   <si>
     <t>&lt;a href="https://kbroman.org/steps2rr/"&gt;Steps toward reproducible research&lt;/a&gt;</t>
@@ -273,15 +252,6 @@
 Library Consultancy&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Borer, E., Seabloom, E., Jones, M. &amp; Schildhauer, M.*</t>
-  </si>
-  <si>
-    <t>Crystal Lewis*</t>
-  </si>
-  <si>
-    <t>Kline, et al.</t>
-  </si>
-  <si>
     <t>&lt;a href="https://docs.google.com/document/d/1u8o5jnWk0Iqp_J06PTu5NjBfVsdoPbBhstht6W0fFp0/edit#heading=h.qjnqq8b54i1d"&gt;Psych-DS: A Technical Specification for Psychological Datasets&lt;/a&gt;</t>
   </si>
   <si>
@@ -291,9 +261,6 @@
     <t>&lt;a href="https://figshare.com/articles/preprint/The_Basics_of_Data_Management/13215350"&gt;The Basics of Data Management&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Reynolds, T., Schatschneider, C. &amp; Logan, J.*</t>
-  </si>
-  <si>
     <t>Search "data management" in repository databases for great resources</t>
   </si>
   <si>
@@ -348,12 +315,6 @@
     <t>Borghi, J., Abrams, S., Lowenberg, D., Simms, S. &amp; Chodacki, J.</t>
   </si>
   <si>
-    <t>Johns Hopkins Institute for Clinical and Translational Research (ICTR)</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://ictrweb.johnshopkins.edu/ictr/dmig/Best_Practice/home.html?v=65849"&gt;Best Practices for Research Data Management&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>J-PAL</t>
   </si>
   <si>
@@ -369,9 +330,6 @@
     <t>&lt;a href="https://doi.org/10.3897/rio.4.e26439"&gt;Support Your Data: A Research Data Management Guide for Researchers&lt;/a&gt;</t>
   </si>
   <si>
-    <t>J-Pal*</t>
-  </si>
-  <si>
     <t>Urban Institute</t>
   </si>
   <si>
@@ -408,13 +366,91 @@
     <t>&lt;a href="https://cghlewis.com/talk/uhcl/"&gt;Data Management Workflows for Education Research Studies&lt;/a&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Crystal Lewis </t>
-  </si>
-  <si>
-    <t>&lt;a href="https://cghlewis.com/blog/data_clean_01/"&gt;Data Cleaning for Data Sharing&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://drive.google.com/drive/folders/1lRKEx_uMhbzcLeVZZBPX6_amde5uYuvf"&gt;Checklists&lt;/a&gt;</t>
+    <t>&lt;a href="https://cghlewis.com/blog/data_clean_01/"&gt;Data Cleaning for Data Sharing Blog Post&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://cghlewis.github.io/ncme-data-cleaning-workshop/"&gt;Data Cleaning for Data Sharing Workshop Materials&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://datamgmtinedresearch.com/"&gt;Data Management in Large-Scale Education Research Book&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://the-turing-way.netlify.app/welcome"&gt;Handbook&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://osf.io/e5g6t/"&gt;Checklists for every phase of a project&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://prezi.com/p/mku89urakpnn/systematic-data-validation/"&gt;Data Validation&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Briney, K.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broman, K.  </t>
+  </si>
+  <si>
+    <t>DeCoster, J.</t>
+  </si>
+  <si>
+    <t>Data Structure Standard</t>
+  </si>
+  <si>
+    <t>Schatschneider, C., Edwards, A., &amp; Shero, J.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://figshare.com/articles/preprint/De-Identification_Guide/13228664/2"&gt;De-identification Guide&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Wilson, et al.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1005510"&gt;Good Enough Practices in Scientific Computing&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>DIME Analytics</t>
+  </si>
+  <si>
+    <t>Filip, A.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.sjsu.edu/research/docs/irb-data-management-handbook.pdf"&gt;Data Management Handbook for Human Subjects Research&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Yenni, et al.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://journals.plos.org/plosbiology/article?id=10.1371/journal.pbio.3000125"&gt;Developing a modern data workflow for regularly updated data&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>J-Pal</t>
+  </si>
+  <si>
+    <t>White, et al.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://ojs.library.queensu.ca/index.php/IEE/article/view/4608"&gt;Nine simple ways to make it easier to (re)use your data&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Towse, A., Ellis, D., Towse, J.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.tandfonline.com/doi/full/10.1080/00224545.2021.1938811"&gt;Making data meaningful: guidelines for good quality open data&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Responsible Data</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://responsibledata.io/resources/handbook/"&gt;The Handbook of the Modern Development Specialist&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://dimewiki.worldbank.org/Main_Page"&gt;DIME Wiki&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>POWER Data Management Hub</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://osf.io/ap3tk/"&gt;Slides from hub presenters&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -769,107 +805,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
+      <c r="B12" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
-    <sortCondition ref="A2:A10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B12">
+    <sortCondition ref="A2:A12"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
-    <hyperlink ref="B10" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
-    <hyperlink ref="B9" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
-    <hyperlink ref="B8" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{17E17D06-812D-4223-9000-D327BBFA127E}"/>
-    <hyperlink ref="B5" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
+    <hyperlink ref="B12" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
+    <hyperlink ref="B11" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
+    <hyperlink ref="B8" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
+    <hyperlink ref="B3" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{D22F0176-8B44-4C40-AF7C-4A1A2E32B8B4}"/>
+    <hyperlink ref="B5" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{EF7E737D-19B2-4BBC-83BA-8A78418603AB}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{3B35D87F-70F7-4DF3-BECE-762D44177028}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -881,82 +935,82 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.453125" customWidth="1"/>
-    <col min="2" max="2" width="64.81640625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -983,163 +1037,163 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="33.54296875" customWidth="1"/>
-    <col min="3" max="3" width="170.7265625" customWidth="1"/>
+    <col min="1" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="170.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>2021</v>
       </c>
       <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>2022</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4">
+        <v>2018</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8">
+        <v>2016</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>2022</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3">
-        <v>2009</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4">
-        <v>2022</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>2021</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5">
-        <v>2018</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2021</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2020</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8">
-        <v>2020</v>
-      </c>
-      <c r="C8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9">
-        <v>2016</v>
-      </c>
-      <c r="C9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10">
-        <v>2022</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>29</v>
       </c>
       <c r="B11">
         <v>2021</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="B12">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
-    <sortCondition ref="A2:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C11">
+    <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{BFC51063-B290-47C9-BA90-DDEEABDB6F04}"/>
-    <hyperlink ref="C7" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{DC152A6E-AD02-4439-B8DA-F74C8A1774B9}"/>
-    <hyperlink ref="C11" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{C2CCC9A4-192D-4723-A6B9-1DD8433A4B7B}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{BFC51063-B290-47C9-BA90-DDEEABDB6F04}"/>
+    <hyperlink ref="C6" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{DC152A6E-AD02-4439-B8DA-F74C8A1774B9}"/>
+    <hyperlink ref="C10" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{C2CCC9A4-192D-4723-A6B9-1DD8433A4B7B}"/>
     <hyperlink ref="C2" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{B8D202EC-299D-4309-9408-24451F78CCC9}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8D4746FE-F3B6-4A3D-ACCA-FFB9D32CE5CF}"/>
-    <hyperlink ref="C10" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{FFCD0CA1-5CD9-45D3-A226-A36829343339}"/>
-    <hyperlink ref="C12" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{1E20410E-725C-4F71-8819-F507842316CA}"/>
-    <hyperlink ref="C3" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{682A5ACB-614C-4F2A-BE8C-8ACBB7384DE1}"/>
-    <hyperlink ref="C8" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{64132426-ED00-4A25-8720-0CBAF1564A6A}"/>
-    <hyperlink ref="C9" r:id="rId10" display="https://rdmkit.elixir-europe.org/" xr:uid="{206910D2-EE19-4E82-989E-46F2C4254F4A}"/>
-    <hyperlink ref="C5" r:id="rId11" display="https://rdmkit.elixir-europe.org/" xr:uid="{529A61DE-AC1F-4EC6-90AD-966DB5394FEE}"/>
+    <hyperlink ref="C5" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8D4746FE-F3B6-4A3D-ACCA-FFB9D32CE5CF}"/>
+    <hyperlink ref="C9" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{FFCD0CA1-5CD9-45D3-A226-A36829343339}"/>
+    <hyperlink ref="C11" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{1E20410E-725C-4F71-8819-F507842316CA}"/>
+    <hyperlink ref="C7" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{64132426-ED00-4A25-8720-0CBAF1564A6A}"/>
+    <hyperlink ref="C8" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{206910D2-EE19-4E82-989E-46F2C4254F4A}"/>
+    <hyperlink ref="C4" r:id="rId10" display="https://rdmkit.elixir-europe.org/" xr:uid="{529A61DE-AC1F-4EC6-90AD-966DB5394FEE}"/>
+    <hyperlink ref="C12" r:id="rId11" display="https://rdmkit.elixir-europe.org/" xr:uid="{A17A33C1-790D-41EB-9DA4-9C2579AE1D3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1147,73 +1201,82 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E314F75B-5804-4835-9447-15ECE75CB0EC}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{DB660BFF-32D8-4552-ADE1-A22912433FF8}"/>
-    <hyperlink ref="B6" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{57D36F4D-5ECB-424B-8CAE-D6BD44420EF1}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{F9369E95-DB00-415B-9C4E-26398D2D43ED}"/>
-    <hyperlink ref="B3" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{31BEDC47-DAD5-48A5-9285-FE7C7BAF828A}"/>
-    <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{F2BB4DDC-F382-4471-AE08-8FFB6600BC49}"/>
+    <hyperlink ref="B6" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{DB660BFF-32D8-4552-ADE1-A22912433FF8}"/>
+    <hyperlink ref="B2" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{57D36F4D-5ECB-424B-8CAE-D6BD44420EF1}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{F9369E95-DB00-415B-9C4E-26398D2D43ED}"/>
+    <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{31BEDC47-DAD5-48A5-9285-FE7C7BAF828A}"/>
+    <hyperlink ref="B3" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{F2BB4DDC-F382-4471-AE08-8FFB6600BC49}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{D7E37755-9937-447D-B08A-D8A38C20E831}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1223,62 +1286,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF00AE3-BFD4-438F-8990-251D0720E643}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1289,8 +1352,8 @@
     <hyperlink ref="B6" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{FA35CA7A-1BB9-4222-B36D-6AA4AF1AFB40}"/>
     <hyperlink ref="B5" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{4AAD8AF4-DD2A-4FBD-BD12-663C4FCEE09D}"/>
     <hyperlink ref="B3" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{09326CED-43A5-4B07-8756-EC90B5BA4D4A}"/>
-    <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{AEB48163-745F-49B3-AAFA-B775BED64A89}"/>
-    <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{7CFA00F0-7017-4EE8-ACA3-9DA1BA5BF9EB}"/>
+    <hyperlink ref="B2" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{AEB48163-745F-49B3-AAFA-B775BED64A89}"/>
+    <hyperlink ref="B4" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{7CFA00F0-7017-4EE8-ACA3-9DA1BA5BF9EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1298,94 +1361,103 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83599360-7CC5-4FEC-96E9-4F9BDB149781}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
       <c r="B2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>91</v>
-      </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
-    <sortCondition ref="A2:A7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
+    <sortCondition ref="A2:A8"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{90272032-5A67-4990-B442-C6BD8299E43E}"/>
+    <hyperlink ref="B6" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{90272032-5A67-4990-B442-C6BD8299E43E}"/>
     <hyperlink ref="B2" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{D8EC5363-580E-427B-B7D1-0E9DDFAEC174}"/>
-    <hyperlink ref="B7" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{BCF07CDC-44C2-4BC3-A669-49A65B574C1A}"/>
+    <hyperlink ref="B8" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{BCF07CDC-44C2-4BC3-A669-49A65B574C1A}"/>
     <hyperlink ref="B3" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{7E3B9977-AC69-49A1-ABF4-47BB4499BAB1}"/>
-    <hyperlink ref="B8" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{E1A2CF24-262B-426D-BD8E-FD5C95E7EDDC}"/>
-    <hyperlink ref="B4" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{967C7D96-CFB3-4000-AFED-F0210BC4FE4E}"/>
-    <hyperlink ref="B6" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{C62F1CA3-935E-41C9-9AB7-B20FAA337BEC}"/>
+    <hyperlink ref="B9" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{E1A2CF24-262B-426D-BD8E-FD5C95E7EDDC}"/>
+    <hyperlink ref="B5" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{967C7D96-CFB3-4000-AFED-F0210BC4FE4E}"/>
+    <hyperlink ref="B7" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{C62F1CA3-935E-41C9-9AB7-B20FAA337BEC}"/>
+    <hyperlink ref="B4" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{7497676C-A29B-4896-B50B-F18E6702CD8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1393,144 +1465,168 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>77</v>
       </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
       <c r="B9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
         <v>108</v>
       </c>
-      <c r="B12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1538,21 +1634,24 @@
     <sortCondition ref="A2:A16"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
-    <hyperlink ref="B11" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{BF5DB17B-A2E9-4364-9EA8-EAFDC95D0D19}"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B7E8A39-208D-4BAB-BD0E-C476EEF71874}"/>
-    <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{17FB9F7C-2EEB-420C-AD50-8F5369FBC4E8}"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
+    <hyperlink ref="B12" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{BF5DB17B-A2E9-4364-9EA8-EAFDC95D0D19}"/>
+    <hyperlink ref="B14" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B7E8A39-208D-4BAB-BD0E-C476EEF71874}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{17FB9F7C-2EEB-420C-AD50-8F5369FBC4E8}"/>
     <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8736C4FB-ED40-4AAA-A513-1B3997C412A1}"/>
-    <hyperlink ref="B13" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
+    <hyperlink ref="B4" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
     <hyperlink ref="B3" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{6400C49C-6A30-43A4-8FD2-3A23E629EA75}"/>
-    <hyperlink ref="B15" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{7497676C-A29B-4896-B50B-F18E6702CD8C}"/>
-    <hyperlink ref="B16" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{58B0795A-28FC-46B1-AAC3-E406B300BDA2}"/>
-    <hyperlink ref="B8" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
-    <hyperlink ref="B12" r:id="rId13" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
-    <hyperlink ref="B7" r:id="rId14" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
-    <hyperlink ref="B6" r:id="rId15" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
+    <hyperlink ref="B9" r:id="rId9" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
+    <hyperlink ref="B5" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
+    <hyperlink ref="B8" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
+    <hyperlink ref="B7" r:id="rId14" display="https://rdmkit.elixir-europe.org/" xr:uid="{9F3CBAC0-B921-4DE2-A65A-B7E86FD49EDC}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://the-turing-way.netlify.app/welcome" xr:uid="{A35D5C69-8E3B-4FAA-9C5E-233488621C17}"/>
+    <hyperlink ref="B19" r:id="rId16" display="https://rdmkit.elixir-europe.org/" xr:uid="{F7DC8ACB-8501-4D8A-8D18-362905B75F1D}"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://the-turing-way.netlify.app/welcome" xr:uid="{8D02884E-C75F-488F-B501-3D966342F33D}"/>
+    <hyperlink ref="B17" r:id="rId18" display="https://rdmkit.elixir-europe.org/" xr:uid="{C98846A5-CA26-45F3-ACCE-26115E7B9672}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1563,61 +1662,61 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" customWidth="1"/>
-    <col min="2" max="2" width="42.1796875" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new excel blog post, update project beginning post
</commit_message>
<xml_diff>
--- a/public/blog/data_mgmt_resources/resources.xlsx
+++ b/public/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5943AD0-C51D-4071-BC05-143EE1AE805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9873F238-FA8A-4B4D-AC75-BA231ACDF66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -348,9 +348,6 @@
     <t>Chicago Beyond</t>
   </si>
   <si>
-    <t>&lt;a href="https://chicagobeyond.org/wp-content/uploads/2019/05/ChicagoBeyond_2019Guidebook.pdf"&gt;Why am I always being researched?&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Poverty Action Lab</t>
   </si>
   <si>
@@ -451,14 +448,34 @@
   </si>
   <si>
     <t>&lt;a href="https://osf.io/ap3tk/"&gt;Slides from hub presenters&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://caltechlibrary.github.io/RDMworkbook/"&gt;The Research Data Management Workbook&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Morrow, J.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.slideshare.net/slideshow/brief-introduction-to-the-12-steps-of-evaluagio/26168236#4"&gt;Brief Introduction to the 12 Steps of Evaluation Data Cleaning&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://chicagobeyond.org/insights/philanthropy/why-am-i-always-being-researched/"&gt;Why am I always being researched?&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -486,11 +503,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,15 +823,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -821,106 +839,115 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>122</v>
       </c>
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>90</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B12">
-    <sortCondition ref="A2:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B13">
+    <sortCondition ref="A3:A13"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
-    <hyperlink ref="B12" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
-    <hyperlink ref="B11" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
-    <hyperlink ref="B8" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
-    <hyperlink ref="B3" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{D22F0176-8B44-4C40-AF7C-4A1A2E32B8B4}"/>
-    <hyperlink ref="B5" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{EF7E737D-19B2-4BBC-83BA-8A78418603AB}"/>
-    <hyperlink ref="B10" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{3B35D87F-70F7-4DF3-BECE-762D44177028}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
+    <hyperlink ref="B13" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
+    <hyperlink ref="B12" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
+    <hyperlink ref="B9" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
+    <hyperlink ref="B4" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{D22F0176-8B44-4C40-AF7C-4A1A2E32B8B4}"/>
+    <hyperlink ref="B6" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{EF7E737D-19B2-4BBC-83BA-8A78418603AB}"/>
+    <hyperlink ref="B11" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{3B35D87F-70F7-4DF3-BECE-762D44177028}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -1169,13 +1196,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12">
         <v>2019</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1203,7 +1230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E314F75B-5804-4835-9447-15ECE75CB0EC}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1223,7 +1250,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
@@ -1231,18 +1258,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
         <v>104</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1263,10 +1290,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" t="s">
         <v>134</v>
-      </c>
-      <c r="B7" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1306,7 +1333,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
@@ -1322,10 +1349,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1399,7 +1426,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
@@ -1465,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1530,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
@@ -1511,7 +1538,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
         <v>82</v>
@@ -1527,10 +1554,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1575,7 +1602,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
         <v>87</v>
@@ -1583,55 +1610,63 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" t="s">
         <v>119</v>
       </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
-    <sortCondition ref="A2:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
+    <sortCondition ref="A2:A17"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
@@ -1648,10 +1683,11 @@
     <hyperlink ref="B8" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
     <hyperlink ref="B15" r:id="rId13" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
     <hyperlink ref="B7" r:id="rId14" display="https://rdmkit.elixir-europe.org/" xr:uid="{9F3CBAC0-B921-4DE2-A65A-B7E86FD49EDC}"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://the-turing-way.netlify.app/welcome" xr:uid="{A35D5C69-8E3B-4FAA-9C5E-233488621C17}"/>
-    <hyperlink ref="B19" r:id="rId16" display="https://rdmkit.elixir-europe.org/" xr:uid="{F7DC8ACB-8501-4D8A-8D18-362905B75F1D}"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://the-turing-way.netlify.app/welcome" xr:uid="{8D02884E-C75F-488F-B501-3D966342F33D}"/>
-    <hyperlink ref="B17" r:id="rId18" display="https://rdmkit.elixir-europe.org/" xr:uid="{C98846A5-CA26-45F3-ACCE-26115E7B9672}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://the-turing-way.netlify.app/welcome" xr:uid="{A35D5C69-8E3B-4FAA-9C5E-233488621C17}"/>
+    <hyperlink ref="B20" r:id="rId16" display="https://rdmkit.elixir-europe.org/" xr:uid="{F7DC8ACB-8501-4D8A-8D18-362905B75F1D}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://the-turing-way.netlify.app/welcome" xr:uid="{8D02884E-C75F-488F-B501-3D966342F33D}"/>
+    <hyperlink ref="B18" r:id="rId18" display="https://rdmkit.elixir-europe.org/" xr:uid="{C98846A5-CA26-45F3-ACCE-26115E7B9672}"/>
+    <hyperlink ref="B16" r:id="rId19" display="https://rdmkit.elixir-europe.org/" xr:uid="{D1FE705A-5C82-4CEA-B5B3-935144D31425}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1662,7 +1698,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,7 +1720,7 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1697,10 +1733,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
         <v>102</v>
-      </c>
-      <c r="B4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>